<commit_message>
modify UserMaster n Forms ctrl
</commit_message>
<xml_diff>
--- a/Uploads/IMOcrewlistForm5.xlsx
+++ b/Uploads/IMOcrewlistForm5.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24228"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F4B589C-4347-4557-A645-523368D4EDBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3738783A-6ED4-4D9C-93FF-7DB3691BA65A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="108" yWindow="96" windowWidth="22932" windowHeight="12264" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>CREW LIST</t>
   </si>
@@ -32,13 +32,19 @@
     <t>Email</t>
   </si>
   <si>
-    <t>Supratik Das</t>
-  </si>
-  <si>
-    <t>Master</t>
-  </si>
-  <si>
-    <t>sup@mail.com</t>
+    <t>amitbh</t>
+  </si>
+  <si>
+    <t>Scond Officer</t>
+  </si>
+  <si>
+    <t>abc@gmai.com</t>
+  </si>
+  <si>
+    <t>bingshu</t>
+  </si>
+  <si>
+    <t>Third Officer</t>
   </si>
 </sst>
 </file>
@@ -530,18 +536,18 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.6640625" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" customWidth="1"/>
-    <col min="3" max="3" width="14.88671875" customWidth="1"/>
-    <col min="4" max="4" width="12.109375" customWidth="1"/>
+    <col min="1" max="1" width="6.7109375" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -549,7 +555,7 @@
       <c r="C1" s="13"/>
       <c r="D1" s="13"/>
     </row>
-    <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
@@ -563,7 +569,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -577,15 +583,21 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>2</v>
       </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="10"/>
-    </row>
-    <row r="5" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>3</v>
       </c>
@@ -593,7 +605,7 @@
       <c r="C5" s="7"/>
       <c r="D5" s="10"/>
     </row>
-    <row r="6" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -601,7 +613,7 @@
       <c r="C6" s="8"/>
       <c r="D6" s="10"/>
     </row>
-    <row r="7" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>5</v>
       </c>
@@ -609,7 +621,7 @@
       <c r="C7" s="8"/>
       <c r="D7" s="10"/>
     </row>
-    <row r="8" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>6</v>
       </c>
@@ -617,7 +629,7 @@
       <c r="C8" s="9"/>
       <c r="D8" s="10"/>
     </row>
-    <row r="9" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>7</v>
       </c>
@@ -625,7 +637,7 @@
       <c r="C9" s="9"/>
       <c r="D9" s="10"/>
     </row>
-    <row r="10" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>8</v>
       </c>
@@ -633,7 +645,7 @@
       <c r="C10" s="9"/>
       <c r="D10" s="10"/>
     </row>
-    <row r="11" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>9</v>
       </c>
@@ -641,7 +653,7 @@
       <c r="C11" s="6"/>
       <c r="D11" s="10"/>
     </row>
-    <row r="12" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>10</v>
       </c>
@@ -649,7 +661,7 @@
       <c r="C12" s="6"/>
       <c r="D12" s="10"/>
     </row>
-    <row r="13" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>11</v>
       </c>
@@ -657,7 +669,7 @@
       <c r="C13" s="6"/>
       <c r="D13" s="10"/>
     </row>
-    <row r="14" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>12</v>
       </c>
@@ -665,7 +677,7 @@
       <c r="C14" s="6"/>
       <c r="D14" s="11"/>
     </row>
-    <row r="15" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>13</v>
       </c>
@@ -673,7 +685,7 @@
       <c r="C15" s="6"/>
       <c r="D15" s="10"/>
     </row>
-    <row r="16" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>14</v>
       </c>
@@ -681,7 +693,7 @@
       <c r="C16" s="6"/>
       <c r="D16" s="10"/>
     </row>
-    <row r="17" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>15</v>
       </c>
@@ -689,7 +701,7 @@
       <c r="C17" s="3"/>
       <c r="D17" s="12"/>
     </row>
-    <row r="18" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>16</v>
       </c>
@@ -697,7 +709,7 @@
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
     </row>
-    <row r="19" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>17</v>
       </c>
@@ -705,7 +717,7 @@
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
     </row>
-    <row r="20" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>18</v>
       </c>
@@ -713,7 +725,7 @@
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
     </row>
-    <row r="21" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>19</v>
       </c>
@@ -721,7 +733,7 @@
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
     </row>
-    <row r="22" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -732,7 +744,7 @@
     <mergeCell ref="A1:D1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1" xr:uid="{934058B6-8324-486F-B31F-FC4CC343D14B}"/>
+    <hyperlink ref="D3" r:id="rId1" xr:uid="{45F4C1E7-4291-42B5-AF4D-141BFEC9C19B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="89" orientation="landscape" r:id="rId2"/>

</xml_diff>

<commit_message>
Modify Crew import from Excel (Add new Temporary Crew and the then Insert)
</commit_message>
<xml_diff>
--- a/Uploads/IMOcrewlistForm5.xlsx
+++ b/Uploads/IMOcrewlistForm5.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24430"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3738783A-6ED4-4D9C-93FF-7DB3691BA65A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{929908A7-67D3-4417-8A62-E145FFF6BEDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>CREW LIST</t>
   </si>
@@ -32,19 +32,13 @@
     <t>Email</t>
   </si>
   <si>
-    <t>amitbh</t>
+    <t>Bhuban</t>
   </si>
   <si>
-    <t>Scond Officer</t>
+    <t>Master</t>
   </si>
   <si>
-    <t>abc@gmai.com</t>
-  </si>
-  <si>
-    <t>bingshu</t>
-  </si>
-  <si>
-    <t>Third Officer</t>
+    <t>master@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -536,18 +530,18 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.7109375" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" customWidth="1"/>
+    <col min="1" max="1" width="6.6640625" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" customWidth="1"/>
+    <col min="3" max="3" width="14.88671875" customWidth="1"/>
+    <col min="4" max="4" width="12.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -555,7 +549,7 @@
       <c r="C1" s="13"/>
       <c r="D1" s="13"/>
     </row>
-    <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
@@ -569,7 +563,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -583,21 +577,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>2</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="10"/>
+    </row>
+    <row r="5" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>3</v>
       </c>
@@ -605,7 +593,7 @@
       <c r="C5" s="7"/>
       <c r="D5" s="10"/>
     </row>
-    <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -613,7 +601,7 @@
       <c r="C6" s="8"/>
       <c r="D6" s="10"/>
     </row>
-    <row r="7" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>5</v>
       </c>
@@ -621,7 +609,7 @@
       <c r="C7" s="8"/>
       <c r="D7" s="10"/>
     </row>
-    <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>6</v>
       </c>
@@ -629,7 +617,7 @@
       <c r="C8" s="9"/>
       <c r="D8" s="10"/>
     </row>
-    <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>7</v>
       </c>
@@ -637,7 +625,7 @@
       <c r="C9" s="9"/>
       <c r="D9" s="10"/>
     </row>
-    <row r="10" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>8</v>
       </c>
@@ -645,7 +633,7 @@
       <c r="C10" s="9"/>
       <c r="D10" s="10"/>
     </row>
-    <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>9</v>
       </c>
@@ -653,7 +641,7 @@
       <c r="C11" s="6"/>
       <c r="D11" s="10"/>
     </row>
-    <row r="12" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>10</v>
       </c>
@@ -661,7 +649,7 @@
       <c r="C12" s="6"/>
       <c r="D12" s="10"/>
     </row>
-    <row r="13" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <v>11</v>
       </c>
@@ -669,7 +657,7 @@
       <c r="C13" s="6"/>
       <c r="D13" s="10"/>
     </row>
-    <row r="14" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
         <v>12</v>
       </c>
@@ -677,7 +665,7 @@
       <c r="C14" s="6"/>
       <c r="D14" s="11"/>
     </row>
-    <row r="15" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
         <v>13</v>
       </c>
@@ -685,7 +673,7 @@
       <c r="C15" s="6"/>
       <c r="D15" s="10"/>
     </row>
-    <row r="16" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
         <v>14</v>
       </c>
@@ -693,7 +681,7 @@
       <c r="C16" s="6"/>
       <c r="D16" s="10"/>
     </row>
-    <row r="17" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
         <v>15</v>
       </c>
@@ -701,7 +689,7 @@
       <c r="C17" s="3"/>
       <c r="D17" s="12"/>
     </row>
-    <row r="18" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="2">
         <v>16</v>
       </c>
@@ -709,7 +697,7 @@
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
     </row>
-    <row r="19" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="2">
         <v>17</v>
       </c>
@@ -717,7 +705,7 @@
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
     </row>
-    <row r="20" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="2">
         <v>18</v>
       </c>
@@ -725,7 +713,7 @@
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
     </row>
-    <row r="21" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="2">
         <v>19</v>
       </c>
@@ -733,7 +721,7 @@
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
     </row>
-    <row r="22" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="2"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -744,7 +732,7 @@
     <mergeCell ref="A1:D1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1" xr:uid="{45F4C1E7-4291-42B5-AF4D-141BFEC9C19B}"/>
+    <hyperlink ref="D3" r:id="rId1" xr:uid="{6FF49AA4-AF5C-4EC9-8AF0-6C881B4D1B3E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="89" orientation="landscape" r:id="rId2"/>

</xml_diff>